<commit_message>
updated data source info
</commit_message>
<xml_diff>
--- a/chart/scatter-chart-tableau/ct-districts-income-grades-2009-13.xlsx
+++ b/chart/scatter-chart-tableau/ct-districts-income-grades-2009-13.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdougherty/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdougherty/Documents/GitHub/datavizforall/chart/scatter-chart-tableau/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="18540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19880" windowHeight="18540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
   <si>
     <t>Andover School District</t>
   </si>
@@ -559,12 +559,6 @@
     <t>Data sources:</t>
   </si>
   <si>
-    <t>Stanford Education Data Archives, TrendCT, ACS 2009-13</t>
-  </si>
-  <si>
-    <t>grade levels =  average of 6th grade English and Math scores on CT tests, linked to NAEP test scores, and expressed as "grade equivalents" (above or below national average), from TrendCT data repository, based on Stanford Education Data Archive</t>
-  </si>
-  <si>
     <t>median household income = American Community Survey 2009-13</t>
   </si>
   <si>
@@ -575,6 +569,18 @@
   </si>
   <si>
     <t>Compiled by Jack Dougherty, Trinity College, March 2017</t>
+  </si>
+  <si>
+    <t>TrendCT, New York Times, Stanford Education Data Archive, American Community Survey 2009-13</t>
+  </si>
+  <si>
+    <t>grade levels =  average of 6th grade English and Math scores on CT tests, linked to NAEP test scores, and expressed as "grade equivalents" (above or below national average), from TrendCT data repository, based on NY Times analysis of Stanford Education Data Archive</t>
+  </si>
+  <si>
+    <t>see more details at</t>
+  </si>
+  <si>
+    <t>https://github.com/jackdougherty/otl-ct-districts-income-grades</t>
   </si>
 </sst>
 </file>
@@ -631,17 +637,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -919,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2609,10 +2618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2628,27 +2637,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
@@ -2688,10 +2697,23 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>